<commit_message>
Added summary file for the second block
Detailed excel file to map reads onto
</commit_message>
<xml_diff>
--- a/raw-data/01-block-1-map.xlsx
+++ b/raw-data/01-block-1-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbf9a23e224bd51a/Documents/GitHub/Chlamydomonas_mic_JRL_2024/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1301" documentId="8_{FB8F087E-4114-4CD7-BBEF-6C25E970F4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C5523A7-2CE2-4C67-A06D-4A80CA042ED8}"/>
+  <xr:revisionPtr revIDLastSave="1302" documentId="8_{FB8F087E-4114-4CD7-BBEF-6C25E970F4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AA88408-CE88-46E7-931D-773F620817E1}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="14" xr2:uid="{80F73A02-C2A8-4BE1-A957-DB27E471ED1A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{80F73A02-C2A8-4BE1-A957-DB27E471ED1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -931,6 +931,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -18267,7 +18271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB5EAEC-7CD0-4338-A5F1-30276D721733}">
   <dimension ref="A1:J1921"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="A1:J1048576"/>
     </sheetView>
   </sheetViews>
@@ -77448,8 +77452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6649A449-5C86-44C8-A944-C1F44E4DDF41}">
   <dimension ref="B1:R20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R20" sqref="A1:R20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>